<commit_message>
Spam Manager (timer and tweet limit)
</commit_message>
<xml_diff>
--- a/la_hacks/Senator Twitter Handles.xlsx
+++ b/la_hacks/Senator Twitter Handles.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\GitHub\LA_Hacks2017\la_hacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,319 +41,319 @@
     <t>Luther Strange</t>
   </si>
   <si>
-    <t>@lutherstrange</t>
-  </si>
-  <si>
     <t>Alaska</t>
   </si>
   <si>
     <t>Lisa Murkowski</t>
   </si>
   <si>
-    <t>@lisamurkowski</t>
-  </si>
-  <si>
     <t>Arizona</t>
   </si>
   <si>
     <t>John McCain</t>
   </si>
   <si>
-    <t>@SenJohnMcCain</t>
-  </si>
-  <si>
     <t>Jeff Flake</t>
   </si>
   <si>
-    <t>@JeffFlake</t>
-  </si>
-  <si>
     <t>Arkansas</t>
   </si>
   <si>
     <t>Tom Cotton</t>
   </si>
   <si>
-    <t>@SenTomCotton</t>
-  </si>
-  <si>
     <t>John Boozman</t>
   </si>
   <si>
-    <t>@JohnBoozman</t>
-  </si>
-  <si>
     <t>Colorado</t>
   </si>
   <si>
     <t>Cory Gardner</t>
   </si>
   <si>
-    <t>@SenCoryGardner</t>
-  </si>
-  <si>
     <t>Florida</t>
   </si>
   <si>
     <t>Marco Rubio</t>
   </si>
   <si>
-    <t>@marcorubio</t>
-  </si>
-  <si>
     <t>Idaho</t>
   </si>
   <si>
     <t>Mike Crapo</t>
   </si>
   <si>
-    <t>@MikeCrapo</t>
-  </si>
-  <si>
     <t>Jim Risch</t>
   </si>
   <si>
-    <t>@SenatorRisch</t>
-  </si>
-  <si>
     <t>Indiana</t>
   </si>
   <si>
     <t>Todd Young</t>
   </si>
   <si>
-    <t>@SenToddYoung</t>
-  </si>
-  <si>
     <t>Iowa</t>
   </si>
   <si>
     <t>Chuck Grassley</t>
   </si>
   <si>
-    <t>@ChuckGrassley</t>
-  </si>
-  <si>
     <t>Joni Ernst</t>
   </si>
   <si>
-    <t>@joniernst</t>
-  </si>
-  <si>
     <t>Kansas</t>
   </si>
   <si>
     <t>Pat Roberts</t>
   </si>
   <si>
-    <t>@SenPatRoberts</t>
-  </si>
-  <si>
     <t>Jerry Moran</t>
   </si>
   <si>
-    <t>@JerryMoran</t>
-  </si>
-  <si>
     <t>Kentucky</t>
   </si>
   <si>
     <t>Mitch McConnell</t>
   </si>
   <si>
-    <t> @SenateMajLdr</t>
-  </si>
-  <si>
     <t>Louisiana</t>
   </si>
   <si>
     <t>Bill Cassidy</t>
   </si>
   <si>
-    <t>@BillCassidy</t>
-  </si>
-  <si>
     <t>Mississippi</t>
   </si>
   <si>
     <t>Thad Cochran</t>
   </si>
   <si>
-    <t>@SenThadCochran</t>
-  </si>
-  <si>
     <t>Roger Wicker</t>
   </si>
   <si>
-    <t>@SenatorWicker</t>
-  </si>
-  <si>
     <t>Missouri</t>
   </si>
   <si>
     <t>Roy Blunt</t>
   </si>
   <si>
-    <t>@RoyBlunt</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
     <t>Steve Daines</t>
   </si>
   <si>
-    <t> @SteveDaines</t>
-  </si>
-  <si>
     <t>Nebraska</t>
   </si>
   <si>
     <t>Deb Fischer</t>
   </si>
   <si>
-    <t>@SenatorFischer</t>
-  </si>
-  <si>
     <t>Nevada</t>
   </si>
   <si>
     <t>Dean Heller</t>
   </si>
   <si>
-    <t>@SenDeanHeller</t>
-  </si>
-  <si>
     <t>North Carolina</t>
   </si>
   <si>
     <t>Richard Burr</t>
   </si>
   <si>
-    <t>@SenatorBurr</t>
-  </si>
-  <si>
     <t>Thom Tillis</t>
   </si>
   <si>
-    <t>@ThomTillis</t>
-  </si>
-  <si>
     <t>North Dakota</t>
   </si>
   <si>
     <t>John Hoeven</t>
   </si>
   <si>
-    <t>@SenJohnHoeven</t>
-  </si>
-  <si>
     <t>Ohio</t>
   </si>
   <si>
     <t>Rob Portman</t>
   </si>
   <si>
-    <t>@robportman</t>
-  </si>
-  <si>
     <t>Oklahoma</t>
   </si>
   <si>
     <t>James Lankford</t>
   </si>
   <si>
-    <t>@SenatorLankford</t>
-  </si>
-  <si>
     <t>Pennsylvania</t>
   </si>
   <si>
     <t>Pat Toomey</t>
   </si>
   <si>
-    <t>@SenToomey</t>
-  </si>
-  <si>
     <t>South Carolina</t>
   </si>
   <si>
     <t>Lindsey Graham</t>
   </si>
   <si>
-    <t>@GrahamBlog</t>
-  </si>
-  <si>
     <t>Tim Scott</t>
   </si>
   <si>
-    <t>@SenatorTimScott</t>
-  </si>
-  <si>
     <t>South Dakota</t>
   </si>
   <si>
     <t>John Thune</t>
   </si>
   <si>
-    <t>@SenJohnThune</t>
-  </si>
-  <si>
     <t>Texas</t>
   </si>
   <si>
     <t>Ted Cruz</t>
   </si>
   <si>
-    <t>@SenTedCruz</t>
-  </si>
-  <si>
     <t>Utah</t>
   </si>
   <si>
     <t>Mike Lee</t>
   </si>
   <si>
-    <t>@SenMikeLee</t>
-  </si>
-  <si>
     <t>West Virginia</t>
   </si>
   <si>
     <t>Shelley Moore Capito</t>
   </si>
   <si>
-    <t>@SenCapito</t>
-  </si>
-  <si>
     <t>Wisconsin</t>
   </si>
   <si>
     <t>Ron Johnson</t>
   </si>
   <si>
-    <t>@SenRonJohnson</t>
-  </si>
-  <si>
     <t>Wyoming</t>
   </si>
   <si>
     <t>Mike Enzi</t>
   </si>
   <si>
-    <t>@SenatorEnzi</t>
-  </si>
-  <si>
     <t>John Barrasso</t>
   </si>
   <si>
-    <t>@SenJohnBarrasso</t>
+    <t>"@lutherstrange</t>
+  </si>
+  <si>
+    <t>"@lisamurkowski</t>
+  </si>
+  <si>
+    <t>"@SenJohnMcCain</t>
+  </si>
+  <si>
+    <t>"@JeffFlake</t>
+  </si>
+  <si>
+    <t>"@SenTomCotton</t>
+  </si>
+  <si>
+    <t>"@JohnBoozman</t>
+  </si>
+  <si>
+    <t>"@SenCoryGardner</t>
+  </si>
+  <si>
+    <t>"@marcorubio</t>
+  </si>
+  <si>
+    <t>"@MikeCrapo</t>
+  </si>
+  <si>
+    <t>"@SenatorRisch</t>
+  </si>
+  <si>
+    <t>"@SenToddYoung</t>
+  </si>
+  <si>
+    <t>"@ChuckGrassley</t>
+  </si>
+  <si>
+    <t>"@joniernst</t>
+  </si>
+  <si>
+    <t>"@SenPatRoberts</t>
+  </si>
+  <si>
+    <t>"@JerryMoran</t>
+  </si>
+  <si>
+    <t> "@SenateMajLdr</t>
+  </si>
+  <si>
+    <t>"@BillCassidy</t>
+  </si>
+  <si>
+    <t>"@SenThadCochran</t>
+  </si>
+  <si>
+    <t>"@SenatorWicker</t>
+  </si>
+  <si>
+    <t>"@RoyBlunt</t>
+  </si>
+  <si>
+    <t> "@SteveDaines</t>
+  </si>
+  <si>
+    <t>"@SenatorFischer</t>
+  </si>
+  <si>
+    <t>"@SenDeanHeller</t>
+  </si>
+  <si>
+    <t>"@SenatorBurr</t>
+  </si>
+  <si>
+    <t>"@ThomTillis</t>
+  </si>
+  <si>
+    <t>"@SenJohnHoeven</t>
+  </si>
+  <si>
+    <t>"@robportman</t>
+  </si>
+  <si>
+    <t>"@SenatorLankford</t>
+  </si>
+  <si>
+    <t>"@SenToomey</t>
+  </si>
+  <si>
+    <t>"@GrahamBlog</t>
+  </si>
+  <si>
+    <t>"@SenatorTimScott</t>
+  </si>
+  <si>
+    <t>"@SenJohnThune</t>
+  </si>
+  <si>
+    <t>"@SenTedCruz</t>
+  </si>
+  <si>
+    <t>"@SenMikeLee</t>
+  </si>
+  <si>
+    <t>"@SenCapito</t>
+  </si>
+  <si>
+    <t>"@SenRonJohnson</t>
+  </si>
+  <si>
+    <t>"@SenatorEnzi</t>
+  </si>
+  <si>
+    <t>"@SenJohnBarrasso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -453,8 +453,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -765,19 +793,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.59765625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.06640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" style="2"/>
-    <col min="5" max="5" width="18.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.59765625" style="2"/>
+    <col min="1" max="1" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="16.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -810,531 +838,650 @@
         <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="D3" s="4" t="str">
+        <f>CONCATENATE(C3, """,")</f>
+        <v>"@lutherstrange",</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1">
+    <row r="4" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <f t="shared" ref="D4:D40" si="0">CONCATENATE(C4, """,")</f>
+        <v>"@lisamurkowski",</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1">
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A5" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenJohnMcCain",</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1">
+    <row r="6" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@JeffFlake",</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1">
+    <row r="7" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A7" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenTomCotton",</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1">
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A8" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@JohnBoozman",</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1">
+    <row r="9" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenCoryGardner",</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@marcorubio",</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" s="6" customFormat="1">
+    <row r="11" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A11" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@MikeCrapo",</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1">
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A12" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorRisch",</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" s="6" customFormat="1">
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A13" s="8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenToddYoung",</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" s="6" customFormat="1">
+    <row r="14" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@ChuckGrassley",</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" s="6" customFormat="1">
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A15" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@joniernst",</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" s="6" customFormat="1">
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenPatRoberts",</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" s="6" customFormat="1">
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@JerryMoran",</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" s="6" customFormat="1">
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v> "@SenateMajLdr",</v>
+      </c>
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1">
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@BillCassidy",</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" s="6" customFormat="1">
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A20" s="8" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenThadCochran",</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" s="6" customFormat="1">
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A21" s="8" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorWicker",</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" s="6" customFormat="1">
+    <row r="22" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A22" s="8" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@RoyBlunt",</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" s="6" customFormat="1">
+    <row r="23" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A23" s="8" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v> "@SteveDaines",</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" s="6" customFormat="1">
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A24" s="8" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorFischer",</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" s="6" customFormat="1">
+    <row r="25" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A25" s="8" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenDeanHeller",</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" s="6" customFormat="1">
+    <row r="26" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A26" s="8" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorBurr",</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" s="6" customFormat="1">
+    <row r="27" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A27" s="8" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@ThomTillis",</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" s="6" customFormat="1">
+    <row r="28" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A28" s="8" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenJohnHoeven",</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" s="6" customFormat="1">
+    <row r="29" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A29" s="8" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="D29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@robportman",</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" s="6" customFormat="1">
+    <row r="30" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A30" s="8" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorLankford",</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" s="6" customFormat="1">
+    <row r="31" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A31" s="8" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="D31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenToomey",</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" s="6" customFormat="1">
+    <row r="32" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A32" s="8" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@GrahamBlog",</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" s="6" customFormat="1">
+    <row r="33" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A33" s="8" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="D33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorTimScott",</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" s="6" customFormat="1">
+    <row r="34" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A34" s="8" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenJohnThune",</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" s="6" customFormat="1">
+    <row r="35" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A35" s="8" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="D35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenTedCruz",</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" s="6" customFormat="1">
+    <row r="36" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A36" s="8" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenMikeLee",</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" s="6" customFormat="1">
+    <row r="37" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A37" s="8" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="4"/>
+        <v>104</v>
+      </c>
+      <c r="D37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenCapito",</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" s="6" customFormat="1">
+    <row r="38" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A38" s="8" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="4"/>
+        <v>105</v>
+      </c>
+      <c r="D38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenRonJohnson",</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" s="6" customFormat="1">
+    <row r="39" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A39" s="8" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="D39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenatorEnzi",</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" s="6" customFormat="1">
+    <row r="40" spans="1:6" s="6" customFormat="1" ht="30">
       <c r="A40" s="8" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="4"/>
+      <c r="D40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>"@SenJohnBarrasso",</v>
+      </c>
       <c r="E40" s="5"/>
     </row>
   </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="D3" sheet="Sheet1"/>
+    </dataRefs>
+  </dataConsolidate>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>